<commit_message>
Questions for mr. Van Peteghem
</commit_message>
<xml_diff>
--- a/Figurenlijst.xlsx
+++ b/Figurenlijst.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andreas Lauwers\Projecten1_ProjectenWebsite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0398155-36C6-4EE1-AEA8-05EACA59EBB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B8DCB4-3200-4755-8775-43A04020783D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4953A3BD-F5F4-493C-9115-6DA7231A6DBB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Figuur 1</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Figuur 3</t>
   </si>
   <si>
-    <t>Resultaten enquête: Hoe heb u uw projectgroep gevonden?</t>
-  </si>
-  <si>
     <t>Figuur 4</t>
   </si>
   <si>
@@ -151,6 +148,72 @@
   </si>
   <si>
     <t>Wireframe Belbin test</t>
+  </si>
+  <si>
+    <t>Codefragment 1</t>
+  </si>
+  <si>
+    <t>Codefragment 2</t>
+  </si>
+  <si>
+    <t>Codefragment 3</t>
+  </si>
+  <si>
+    <t>Codefragment 4</t>
+  </si>
+  <si>
+    <t>Codefragment 5</t>
+  </si>
+  <si>
+    <t>Codefragment 6</t>
+  </si>
+  <si>
+    <t>Codefragment 7</t>
+  </si>
+  <si>
+    <t>Codefragment 8</t>
+  </si>
+  <si>
+    <t>Codefragment 9</t>
+  </si>
+  <si>
+    <t>Screenshot oude projectenwebsite</t>
+  </si>
+  <si>
+    <t>PHP artisan make commando</t>
+  </si>
+  <si>
+    <t>Databankmodel projectenwebsite</t>
+  </si>
+  <si>
+    <t>Uitvoeren van migrating en seeding</t>
+  </si>
+  <si>
+    <t>Seederbestand gebruikers</t>
+  </si>
+  <si>
+    <t>Migrationbestand gebruikers</t>
+  </si>
+  <si>
+    <t>Eloquent model student</t>
+  </si>
+  <si>
+    <t>Controller van overzichten</t>
+  </si>
+  <si>
+    <t>Nazien of een gebruiker ingelogd is m.b.v. Bladeparameters</t>
+  </si>
+  <si>
+    <t>Routes</t>
+  </si>
+  <si>
+    <t>Figuur 21</t>
+  </si>
+  <si>
+    <t>Figuur 22</t>
+  </si>
+  <si>
+    <t>Resultaten enquête: Hoe hebt u uw projectgroep gevonden?</t>
   </si>
 </sst>
 </file>
@@ -502,237 +565,419 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B500BA-6CE5-4DB6-A414-FA7FC749E282}">
-  <dimension ref="E8:G28"/>
+  <dimension ref="E8:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G41" sqref="E34:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>0</v>
       </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
       <c r="G8">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="G9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>4</v>
       </c>
       <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
         <v>3</v>
       </c>
-      <c r="G10">
+      <c r="G11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <f>H13+10</f>
+        <v>29</v>
+      </c>
+      <c r="H13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G29" si="0">H14+10</f>
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="H15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="H19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="H20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="H21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="H22">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="H23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="H24">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="H26">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="H27">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="H28">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35">
         <v>14</v>
       </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37">
         <v>16</v>
       </c>
-      <c r="F16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" t="s">
+        <v>54</v>
+      </c>
+      <c r="G38">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" t="s">
+        <v>55</v>
+      </c>
+      <c r="G39">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40">
         <v>18</v>
       </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" t="s">
-        <v>37</v>
-      </c>
-      <c r="G27">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
-        <v>39</v>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>